<commit_message>
ny_versjon_23022021 - særskilt skatteplikt inn i egenskap_objekt_felt.xlsx
</commit_message>
<xml_diff>
--- a/docs/documentation/informasjonsmodell/egenskap_objekt_felt.xlsx
+++ b/docs/documentation/informasjonsmodell/egenskap_objekt_felt.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k89414\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\github\skattemeldingen\docs\documentation\informasjonsmodell\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="39915" windowHeight="14340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
-    <sheet name="Ark3" sheetId="3" r:id="rId3"/>
+    <sheet name="Ark3" sheetId="4" r:id="rId3"/>
+    <sheet name="Ark3_old" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="317">
   <si>
     <t>Tema</t>
   </si>
@@ -758,6 +759,228 @@
   </si>
   <si>
     <t>Kan: renteinntektAvObligasjonOgSertifikat, NY: Kan: skattepliktigGevinstVedRealisasjonAvObligasjonOgSertifikat, Kan: skattepliktigTapVedRealisasjonAvObligasjonOgSertifikat</t>
+  </si>
+  <si>
+    <t>Undertema</t>
+  </si>
+  <si>
+    <t>Detaljer på undertema</t>
+  </si>
+  <si>
+    <t>Sette kommune på objekt</t>
+  </si>
+  <si>
+    <t>Sette særskilt skatteplikt på objekt</t>
+  </si>
+  <si>
+    <t>Lønn og tilsvarende ytelser (inkl godtgjørelser) inkl Særskilt fradrag for sjøfolk</t>
+  </si>
+  <si>
+    <t>KPL skattepliktSomUtenrikstjenestemann skattepliktEtterPetroleumsskatteloven skattepliktSomSjoemann skattepliktAvNaeringsdriftEiendomMv</t>
+  </si>
+  <si>
+    <t>skattepliktSomUtenrikstjenestemann skattepliktEtterPetroleumsskatteloven skattepliktSomSjoemann</t>
+  </si>
+  <si>
+    <t>skattepliktSomUtenrikstjenestemann skattepliktEtterPetroleumsskatteloven</t>
+  </si>
+  <si>
+    <t>NY kan:  kreverAvstandsfradragVedBrukAvEgenBilForBesoeksreiseTilHjemmetUtenforEOeS</t>
+  </si>
+  <si>
+    <t>Ny Kan:dokumenterteKostnaderTilKost, Ny Kan:dokumenterteKostnaderTilKostUtoverMottattKostgodtgjoerelse, Ny Kan:dokumenterteKostnaderTilLosji</t>
+  </si>
+  <si>
+    <t>skattepliktSomUtenrikstjenestemann</t>
+  </si>
+  <si>
+    <t>Kostnader knyttet til arbeid og andre inntekter</t>
+  </si>
+  <si>
+    <t>Kostnader knyttet til arbeid og andre inntekter og minstefradrag</t>
+  </si>
+  <si>
+    <t>Minstefradrag ektefelletillegg</t>
+  </si>
+  <si>
+    <t>Minstefradrag barnepensjon</t>
+  </si>
+  <si>
+    <t>Annen arbeidsinntekt</t>
+  </si>
+  <si>
+    <t>Annen arbeidsinntekt (inkl personinntekt)</t>
+  </si>
+  <si>
+    <t>skattepliktSomUtenrikstjenestemann skattepliktAvNaeringsdriftEiendomMv</t>
+  </si>
+  <si>
+    <t>Annen arbeidsinntekt fra fisk</t>
+  </si>
+  <si>
+    <t>skattepliktSomUtenrikstjenestemann kildeskattepliktPaaPensjon</t>
+  </si>
+  <si>
+    <t>10% standardfradrag</t>
+  </si>
+  <si>
+    <t>skattepliktEtterPetroleumsskatteloven skattepliktSomSjoemann</t>
+  </si>
+  <si>
+    <t>Bank, lån og forsikring</t>
+  </si>
+  <si>
+    <t>skattepliktSomUtenrikstjenestemann skattepliktAvNaeringsdriftEiendomMv skattepliktEtterPetroleumsskatteloven</t>
+  </si>
+  <si>
+    <t>skattepliktAvNaeringsdriftEiendomMv skattepliktSomUtenrikstjenestemann</t>
+  </si>
+  <si>
+    <t>Andre kapitalkostnader</t>
+  </si>
+  <si>
+    <t>skattepliktAvNaeringsdriftEiendomMv</t>
+  </si>
+  <si>
+    <t>Tilleggseiendommer</t>
+  </si>
+  <si>
+    <t>NY: Kan:  vedlikeholdskostnadVedUtleie OG annenKostnadVedUtleie</t>
+  </si>
+  <si>
+    <t>NY: Kan: vedlikeholdskostnadVedUtleie OG annenKostnadVedUtleie</t>
+  </si>
+  <si>
+    <t>s kattepliktSomUtenrikstjenestemann skattepliktAvNaeringsdriftEiendomMv</t>
+  </si>
+  <si>
+    <t>Kapitalisert festeavgift</t>
+  </si>
+  <si>
+    <t>Ny Kan: Betalt barnepass - betaltBeloep</t>
+  </si>
+  <si>
+    <t>Ny kan: faktiskKostnadForMerkjoeringForAaBringeOgHenteBarn,</t>
+  </si>
+  <si>
+    <t>Særfradrag store sykdomskostnader</t>
+  </si>
+  <si>
+    <t>Særfradrag liten ervervsevne</t>
+  </si>
+  <si>
+    <t>Finans</t>
+  </si>
+  <si>
+    <t>NY: Kan: skattepliktigGevinstVedRealisasjon, NY: Kan: skattepliktigTapVedRealisasjon, NY: Kan: verdiFoerVerdsettingsrabattForAksjedel, NY: Kan: formuesverdiForKontanter</t>
+  </si>
+  <si>
+    <t>NY: Kan: skattepliktigTapVedRealisasjonAvAndelIAksjedel, NY: Kan:skattepliktigTapVedRealisasjonAvAndelIRentedel, NY: Kan:skattepliktigGevinstVedRealisasjonAvAndelIAksjedel, NY: Kan:skattepliktigGevinstVedRealisasjonAvAndelIRentedel, NY: Kan:skattepliktigUtbytte, NY: Kan:skattepliktigRenteinntekt</t>
+  </si>
+  <si>
+    <t>NY: Kan: renteinntektAvObligasjonOgSertifikat, NY: Kan: skattepliktigGevinstVedRealisasjonAvObligasjonOgSertifikat, NY: Kan: skattepliktigTapVedRealisasjonAvObligasjonOgSertifikat</t>
+  </si>
+  <si>
+    <t>skattepliktAvNaeringsdriftEiendomMv skattepliktSomUtenrikstjenestemann skattepliktEtterPetroleumsskatteloven</t>
+  </si>
+  <si>
+    <t>Skattepliktsinformasjon</t>
+  </si>
+  <si>
+    <t>Kildeskatt på pensjon, dokumentasjoon om bostedsland og skatteavtale</t>
+  </si>
+  <si>
+    <t>Skattebegrensing §17.1</t>
+  </si>
+  <si>
+    <t>Skattebegrensing §17.4</t>
+  </si>
+  <si>
+    <t>ja (ikke mulig å fordele til flere kommuner i pilot)</t>
+  </si>
+  <si>
+    <t>Vergegodtgjørelse</t>
+  </si>
+  <si>
+    <t>Næring</t>
+  </si>
+  <si>
+    <t>Næringsinntekt mv</t>
+  </si>
+  <si>
+    <t>Næringsinntekt/sykepenger fra a-melding</t>
+  </si>
+  <si>
+    <t>Næringsinntekt mv, fordelt fra ektefelle</t>
+  </si>
+  <si>
+    <t>Netto formue</t>
+  </si>
+  <si>
+    <t>Netto formue, fordelt fra ektefelle</t>
+  </si>
+  <si>
+    <t>Forenklet næringsopplysninger</t>
+  </si>
+  <si>
+    <t>Inntekt og kostnad for lott og hyremottakere</t>
+  </si>
+  <si>
+    <t>Fradrag i primærnæring</t>
+  </si>
+  <si>
+    <t>Fradrag for jordbruk</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Fradrag for reindrift</t>
+  </si>
+  <si>
+    <t>Fradrag for skiferproduksjon</t>
+  </si>
+  <si>
+    <t>Særskilt fradrag for fiske og fangstfolk</t>
+  </si>
+  <si>
+    <t>4 x kommunefordelingskort</t>
+  </si>
+  <si>
+    <t>Kredittfradrag</t>
+  </si>
+  <si>
+    <t>Betalt skatt i utlandet tidliger e år (fremført skatt)</t>
+  </si>
+  <si>
+    <t>Resultat og mellomberegninger (SMIA)</t>
+  </si>
+  <si>
+    <t>Selskap med deltakerfastsetting</t>
+  </si>
+  <si>
+    <t>Arbeidsgodtgjørelse, pr næring, inkl samordning av negativ personinntekt</t>
+  </si>
+  <si>
+    <t>Inntekter pr næring</t>
+  </si>
+  <si>
+    <t>Egenskaper på objekt</t>
+  </si>
+  <si>
+    <t>Egenskaper på felt</t>
+  </si>
+  <si>
+    <t>Skyldig og til gode underholdsbidrag</t>
+  </si>
+  <si>
+    <t>Andre forhold</t>
+  </si>
+  <si>
+    <t>Metode for å unngå dobbeltbeskatning Kredittfradrag og alternativ fordeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja </t>
   </si>
 </sst>
 </file>
@@ -854,7 +1077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -892,6 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1740,10 +1964,1783 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" customWidth="1"/>
+    <col min="11" max="11" width="54.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D1" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>250</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" t="s">
+        <v>250</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" t="s">
+        <v>253</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" t="s">
+        <v>253</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" t="s">
+        <v>255</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>249</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" t="s">
+        <v>250</v>
+      </c>
+      <c r="G16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" t="s">
+        <v>250</v>
+      </c>
+      <c r="G17" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" t="s">
+        <v>262</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>263</v>
+      </c>
+      <c r="C19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F19" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>266</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" t="s">
+        <v>138</v>
+      </c>
+      <c r="L21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>266</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>266</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" t="s">
+        <v>253</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" t="s">
+        <v>250</v>
+      </c>
+      <c r="G25" t="s">
+        <v>145</v>
+      </c>
+      <c r="H25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" t="s">
+        <v>316</v>
+      </c>
+      <c r="J25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" t="s">
+        <v>250</v>
+      </c>
+      <c r="H26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" t="s">
+        <v>250</v>
+      </c>
+      <c r="H27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" t="s">
+        <v>250</v>
+      </c>
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" t="s">
+        <v>253</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>267</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>268</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" t="s">
+        <v>313</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
+        <v>269</v>
+      </c>
+      <c r="G34" t="s">
+        <v>152</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
+        <v>152</v>
+      </c>
+      <c r="K34" t="s">
+        <v>153</v>
+      </c>
+      <c r="L34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" t="s">
+        <v>137</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
+        <v>269</v>
+      </c>
+      <c r="H35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>270</v>
+      </c>
+      <c r="D36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" t="s">
+        <v>269</v>
+      </c>
+      <c r="H36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>260</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" t="s">
+        <v>158</v>
+      </c>
+      <c r="L37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>267</v>
+      </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
+        <v>267</v>
+      </c>
+      <c r="G39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>260</v>
+      </c>
+      <c r="L41" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" t="s">
+        <v>260</v>
+      </c>
+      <c r="L42" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" t="s">
+        <v>253</v>
+      </c>
+      <c r="G43" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" t="s">
+        <v>168</v>
+      </c>
+      <c r="L43" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" t="s">
+        <v>260</v>
+      </c>
+      <c r="G44" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>170</v>
+      </c>
+      <c r="D45" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" t="s">
+        <v>253</v>
+      </c>
+      <c r="H45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" t="s">
+        <v>137</v>
+      </c>
+      <c r="F46" t="s">
+        <v>253</v>
+      </c>
+      <c r="G46" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" t="s">
+        <v>18</v>
+      </c>
+      <c r="J46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" t="s">
+        <v>253</v>
+      </c>
+      <c r="G47" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" t="s">
+        <v>137</v>
+      </c>
+      <c r="E48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" t="s">
+        <v>273</v>
+      </c>
+      <c r="G48" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" t="s">
+        <v>274</v>
+      </c>
+      <c r="D49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" t="s">
+        <v>250</v>
+      </c>
+      <c r="H51" t="s">
+        <v>204</v>
+      </c>
+      <c r="J51" t="s">
+        <v>204</v>
+      </c>
+      <c r="L51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>177</v>
+      </c>
+      <c r="D52" t="s">
+        <v>113</v>
+      </c>
+      <c r="H52" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" t="s">
+        <v>18</v>
+      </c>
+      <c r="L52" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" t="s">
+        <v>113</v>
+      </c>
+      <c r="H53" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" t="s">
+        <v>18</v>
+      </c>
+      <c r="L53" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54" t="s">
+        <v>113</v>
+      </c>
+      <c r="H54" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" t="s">
+        <v>113</v>
+      </c>
+      <c r="F55" t="s">
+        <v>250</v>
+      </c>
+      <c r="H55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>277</v>
+      </c>
+      <c r="F56" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>278</v>
+      </c>
+      <c r="F57" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>182</v>
+      </c>
+      <c r="D59" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" t="s">
+        <v>250</v>
+      </c>
+      <c r="H59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" t="s">
+        <v>137</v>
+      </c>
+      <c r="F60" t="s">
+        <v>250</v>
+      </c>
+      <c r="H60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" t="s">
+        <v>18</v>
+      </c>
+      <c r="L60" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>183</v>
+      </c>
+      <c r="D61" t="s">
+        <v>137</v>
+      </c>
+      <c r="F61" t="s">
+        <v>250</v>
+      </c>
+      <c r="G61" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61" t="s">
+        <v>186</v>
+      </c>
+      <c r="L61" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>188</v>
+      </c>
+      <c r="D62" t="s">
+        <v>113</v>
+      </c>
+      <c r="F62" t="s">
+        <v>250</v>
+      </c>
+      <c r="H62" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" t="s">
+        <v>18</v>
+      </c>
+      <c r="L62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>190</v>
+      </c>
+      <c r="D63" t="s">
+        <v>137</v>
+      </c>
+      <c r="F63" t="s">
+        <v>250</v>
+      </c>
+      <c r="G63" t="s">
+        <v>191</v>
+      </c>
+      <c r="H63" t="s">
+        <v>18</v>
+      </c>
+      <c r="I63" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" t="s">
+        <v>18</v>
+      </c>
+      <c r="K63" t="s">
+        <v>192</v>
+      </c>
+      <c r="L63" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" t="s">
+        <v>137</v>
+      </c>
+      <c r="F64" t="s">
+        <v>250</v>
+      </c>
+      <c r="G64" t="s">
+        <v>18</v>
+      </c>
+      <c r="H64" t="s">
+        <v>18</v>
+      </c>
+      <c r="I64" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" t="s">
+        <v>18</v>
+      </c>
+      <c r="K64" t="s">
+        <v>194</v>
+      </c>
+      <c r="L64" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" t="s">
+        <v>137</v>
+      </c>
+      <c r="F65" t="s">
+        <v>253</v>
+      </c>
+      <c r="G65" t="s">
+        <v>18</v>
+      </c>
+      <c r="H65" t="s">
+        <v>18</v>
+      </c>
+      <c r="I65" t="s">
+        <v>18</v>
+      </c>
+      <c r="J65" t="s">
+        <v>18</v>
+      </c>
+      <c r="K65" t="s">
+        <v>196</v>
+      </c>
+      <c r="L65" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>197</v>
+      </c>
+      <c r="D66" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" t="s">
+        <v>283</v>
+      </c>
+      <c r="G66" t="s">
+        <v>18</v>
+      </c>
+      <c r="H66" t="s">
+        <v>18</v>
+      </c>
+      <c r="I66" t="s">
+        <v>18</v>
+      </c>
+      <c r="J66" t="s">
+        <v>18</v>
+      </c>
+      <c r="K66" t="s">
+        <v>198</v>
+      </c>
+      <c r="L66" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D67" t="s">
+        <v>137</v>
+      </c>
+      <c r="F67" t="s">
+        <v>250</v>
+      </c>
+      <c r="G67" t="s">
+        <v>18</v>
+      </c>
+      <c r="H67" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" t="s">
+        <v>18</v>
+      </c>
+      <c r="J67" t="s">
+        <v>18</v>
+      </c>
+      <c r="K67" t="s">
+        <v>198</v>
+      </c>
+      <c r="L67" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>202</v>
+      </c>
+      <c r="C69" t="s">
+        <v>203</v>
+      </c>
+      <c r="D69" t="s">
+        <v>137</v>
+      </c>
+      <c r="F69" t="s">
+        <v>250</v>
+      </c>
+      <c r="G69" t="s">
+        <v>204</v>
+      </c>
+      <c r="H69" t="s">
+        <v>18</v>
+      </c>
+      <c r="I69" t="s">
+        <v>18</v>
+      </c>
+      <c r="J69" t="s">
+        <v>18</v>
+      </c>
+      <c r="L69" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>206</v>
+      </c>
+      <c r="D70" t="s">
+        <v>113</v>
+      </c>
+      <c r="F70" t="s">
+        <v>250</v>
+      </c>
+      <c r="H70" t="s">
+        <v>18</v>
+      </c>
+      <c r="J70" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" t="s">
+        <v>113</v>
+      </c>
+      <c r="H71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>45</v>
+      </c>
+      <c r="D72" t="s">
+        <v>113</v>
+      </c>
+      <c r="H72" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>208</v>
+      </c>
+      <c r="D73" t="s">
+        <v>113</v>
+      </c>
+      <c r="G73" t="s">
+        <v>18</v>
+      </c>
+      <c r="H73" t="s">
+        <v>19</v>
+      </c>
+      <c r="I73" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" t="s">
+        <v>135</v>
+      </c>
+      <c r="D75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F75" t="s">
+        <v>253</v>
+      </c>
+      <c r="G75" t="s">
+        <v>18</v>
+      </c>
+      <c r="H75" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>284</v>
+      </c>
+      <c r="C76" t="s">
+        <v>214</v>
+      </c>
+      <c r="H76" t="s">
+        <v>19</v>
+      </c>
+      <c r="L76" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>216</v>
+      </c>
+      <c r="H77" t="s">
+        <v>19</v>
+      </c>
+      <c r="L77" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>218</v>
+      </c>
+      <c r="H78" t="s">
+        <v>19</v>
+      </c>
+      <c r="L78" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>220</v>
+      </c>
+      <c r="H79" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>286</v>
+      </c>
+      <c r="C81" t="s">
+        <v>286</v>
+      </c>
+      <c r="D81" t="s">
+        <v>113</v>
+      </c>
+      <c r="H81" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>287</v>
+      </c>
+      <c r="C82" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>222</v>
+      </c>
+      <c r="C83" t="s">
+        <v>222</v>
+      </c>
+      <c r="D83" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83" t="s">
+        <v>288</v>
+      </c>
+      <c r="F83" t="s">
+        <v>266</v>
+      </c>
+      <c r="H83" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>289</v>
+      </c>
+      <c r="F84" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>290</v>
+      </c>
+      <c r="C86" t="s">
+        <v>291</v>
+      </c>
+      <c r="E86" t="s">
+        <v>18</v>
+      </c>
+      <c r="F86" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>292</v>
+      </c>
+      <c r="E87" t="s">
+        <v>18</v>
+      </c>
+      <c r="F87" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>293</v>
+      </c>
+      <c r="E88" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>294</v>
+      </c>
+      <c r="E89" t="s">
+        <v>288</v>
+      </c>
+      <c r="F89" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>295</v>
+      </c>
+      <c r="E90" t="s">
+        <v>18</v>
+      </c>
+      <c r="F90" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>296</v>
+      </c>
+      <c r="E91" t="s">
+        <v>18</v>
+      </c>
+      <c r="F91" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>297</v>
+      </c>
+      <c r="E92" t="s">
+        <v>18</v>
+      </c>
+      <c r="F92" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>299</v>
+      </c>
+      <c r="E94" t="s">
+        <v>300</v>
+      </c>
+      <c r="F94" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>301</v>
+      </c>
+      <c r="E95" t="s">
+        <v>300</v>
+      </c>
+      <c r="F95" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>302</v>
+      </c>
+      <c r="E96" t="s">
+        <v>300</v>
+      </c>
+      <c r="F96" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>303</v>
+      </c>
+      <c r="E97" t="s">
+        <v>300</v>
+      </c>
+      <c r="F97" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>304</v>
+      </c>
+      <c r="E98" t="s">
+        <v>18</v>
+      </c>
+      <c r="F98" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>305</v>
+      </c>
+      <c r="C100" t="s">
+        <v>209</v>
+      </c>
+      <c r="D100" t="s">
+        <v>113</v>
+      </c>
+      <c r="G100" t="s">
+        <v>18</v>
+      </c>
+      <c r="H100" t="s">
+        <v>18</v>
+      </c>
+      <c r="I100" t="s">
+        <v>18</v>
+      </c>
+      <c r="L100" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>211</v>
+      </c>
+      <c r="D102" t="s">
+        <v>113</v>
+      </c>
+      <c r="H102" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>212</v>
+      </c>
+      <c r="D103" t="s">
+        <v>113</v>
+      </c>
+      <c r="H103" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>213</v>
+      </c>
+      <c r="D104" t="s">
+        <v>113</v>
+      </c>
+      <c r="H104" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>217</v>
+      </c>
+      <c r="H107" t="s">
+        <v>19</v>
+      </c>
+      <c r="L107" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>219</v>
+      </c>
+      <c r="H108" t="s">
+        <v>19</v>
+      </c>
+      <c r="L108" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>308</v>
+      </c>
+      <c r="C110" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L88" sqref="L88"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,6 +5549,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000EF898EB4470704BB86F1A19A5662393" ma:contentTypeVersion="0" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="2559e4243634f758674830a574aa02fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5eb6cd67344829d3a956a36ab89737e9">
     <xsd:element name="properties">
@@ -3665,15 +5671,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3681,6 +5678,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF91971-B380-4AC3-AD39-3D5F451AA34B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8197AB80-839C-4AE2-9E71-89C97FF1CC4E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3692,14 +5697,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF91971-B380-4AC3-AD39-3D5F451AA34B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>